<commit_message>
Languages separated into lists (mostly)
</commit_message>
<xml_diff>
--- a/mentees.xlsx
+++ b/mentees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepb\Documents\Miscellaneous\Coding\Projects\ISMA matching\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9183B530-F35E-49B7-B114-A3EE112321CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48E0118-A378-48AE-9901-F8EA604F67AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="2085" windowWidth="14400" windowHeight="7495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="2415" windowWidth="14400" windowHeight="7495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -819,9 +819,9 @@
   </sheetPr>
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.6"/>

</xml_diff>